<commit_message>
feat(mineralCroller) : Feat getting chemical formula from wikipedia website by mineral name
</commit_message>
<xml_diff>
--- a/mineralDB.xlsx
+++ b/mineralDB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wontaeyeon/Documents/세종대/2022-1/선광제련공학개론/mineral-price-calculator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{C20A0306-063E-7247-B4D9-0D26FC2F4F9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{A41D11EF-D032-4C43-8AF9-8B715C43394E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5940" yWindow="22100" windowWidth="28800" windowHeight="17500"/>
   </bookViews>
@@ -229,9 +229,6 @@
     <t>Realgar</t>
   </si>
   <si>
-    <t>goethite</t>
-  </si>
-  <si>
     <t>Sapphire</t>
   </si>
   <si>
@@ -256,9 +253,6 @@
     <t>Stibnite</t>
   </si>
   <si>
-    <t>Hermatite</t>
-  </si>
-  <si>
     <t>Magnetite</t>
   </si>
   <si>
@@ -272,6 +266,12 @@
   </si>
   <si>
     <t>Hemimorphite</t>
+  </si>
+  <si>
+    <t>Goethite</t>
+  </si>
+  <si>
+    <t>Hematite</t>
   </si>
 </sst>
 </file>
@@ -1130,7 +1130,7 @@
   <dimension ref="B3:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1172,7 +1172,7 @@
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E5" t="s">
         <v>6</v>
@@ -1209,7 +1209,7 @@
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="E7" t="s">
         <v>14</v>
@@ -1226,7 +1226,7 @@
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E8" t="s">
         <v>16</v>
@@ -1243,7 +1243,7 @@
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E9" t="s">
         <v>18</v>
@@ -1260,7 +1260,7 @@
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E10" t="s">
         <v>19</v>
@@ -1277,7 +1277,7 @@
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E11" t="s">
         <v>21</v>
@@ -1294,7 +1294,7 @@
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E12" t="s">
         <v>23</v>
@@ -1311,7 +1311,7 @@
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E13" t="s">
         <v>25</v>
@@ -1328,7 +1328,7 @@
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E14" t="s">
         <v>28</v>
@@ -1345,7 +1345,7 @@
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E15" t="s">
         <v>32</v>
@@ -1362,7 +1362,7 @@
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="E16" t="s">
         <v>33</v>
@@ -1379,7 +1379,7 @@
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E17" t="s">
         <v>35</v>
@@ -1396,7 +1396,7 @@
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E18" t="s">
         <v>36</v>
@@ -1413,7 +1413,7 @@
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E19" t="s">
         <v>37</v>
@@ -1430,7 +1430,7 @@
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E20" t="s">
         <v>38</v>

</xml_diff>